<commit_message>
Last Order column added to AmazonOrder
</commit_message>
<xml_diff>
--- a/appdata/orderForm.xlsx
+++ b/appdata/orderForm.xlsx
@@ -440,7 +440,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C10"/>
+  <dimension ref="A1:C30"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -468,22 +468,22 @@
     <row r="2">
       <c r="A2" s="2" t="inlineStr">
         <is>
-          <t>AL_NAOMI_T14/88</t>
+          <t>AL_EASY BRAID 18_34</t>
         </is>
       </c>
       <c r="B2" s="2" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C2" s="2" t="inlineStr">
         <is>
-          <t>10397 T14/88</t>
+          <t>14657 34</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="2" t="inlineStr">
         <is>
-          <t>AL_SASHA_1B</t>
+          <t>AL_NAOMI_T14/88</t>
         </is>
       </c>
       <c r="B3" s="2" t="n">
@@ -491,29 +491,29 @@
       </c>
       <c r="C3" s="2" t="inlineStr">
         <is>
-          <t>10521 1B</t>
+          <t>10397 T14/88</t>
         </is>
       </c>
     </row>
     <row r="4">
       <c r="A4" s="2" t="inlineStr">
         <is>
-          <t>BY_KOBY_T27B</t>
+          <t>AL_SASHA_1B</t>
         </is>
       </c>
       <c r="B4" s="2" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C4" s="2" t="inlineStr">
         <is>
-          <t>KOBY</t>
+          <t>10521 1B</t>
         </is>
       </c>
     </row>
     <row r="5">
       <c r="A5" s="2" t="inlineStr">
         <is>
-          <t>BY_STB COGIC_M27/613</t>
+          <t>BY_AUSTIN_SP427</t>
         </is>
       </c>
       <c r="B5" s="2" t="n">
@@ -521,14 +521,14 @@
       </c>
       <c r="C5" s="2" t="inlineStr">
         <is>
-          <t>STB COGIC</t>
+          <t>AUSTIN</t>
         </is>
       </c>
     </row>
     <row r="6">
       <c r="A6" s="2" t="inlineStr">
         <is>
-          <t>HZ_HAYLIE_1B</t>
+          <t>BY_DOLLY_2</t>
         </is>
       </c>
       <c r="B6" s="2" t="n">
@@ -536,14 +536,14 @@
       </c>
       <c r="C6" s="2" t="inlineStr">
         <is>
-          <t>IBBHAY</t>
+          <t>DOLLY</t>
         </is>
       </c>
     </row>
     <row r="7">
       <c r="A7" s="2" t="inlineStr">
         <is>
-          <t>HZ_IDPWKS24_2</t>
+          <t>BY_KOBY_T27B</t>
         </is>
       </c>
       <c r="B7" s="2" t="n">
@@ -551,14 +551,14 @@
       </c>
       <c r="C7" s="2" t="inlineStr">
         <is>
-          <t>IDPWKS24IDPWKS24</t>
+          <t>KOBY</t>
         </is>
       </c>
     </row>
     <row r="8">
       <c r="A8" s="2" t="inlineStr">
         <is>
-          <t>OT_ROLL UP 44PCS_280</t>
+          <t>BY_MALIA_2</t>
         </is>
       </c>
       <c r="B8" s="2" t="n">
@@ -566,14 +566,14 @@
       </c>
       <c r="C8" s="2" t="inlineStr">
         <is>
-          <t>HWVBRU234</t>
+          <t>MALIA</t>
         </is>
       </c>
     </row>
     <row r="9">
       <c r="A9" s="2" t="inlineStr">
         <is>
-          <t>OT_ROLL UP 44PCS_33</t>
+          <t>BY_MATA_SP427</t>
         </is>
       </c>
       <c r="B9" s="2" t="n">
@@ -581,22 +581,322 @@
       </c>
       <c r="C9" s="2" t="inlineStr">
         <is>
-          <t>HWVBRU234</t>
+          <t>MATA</t>
         </is>
       </c>
     </row>
     <row r="10">
       <c r="A10" s="2" t="inlineStr">
         <is>
+          <t>BY_PEDY_SP427</t>
+        </is>
+      </c>
+      <c r="B10" s="2" t="n">
+        <v>1</v>
+      </c>
+      <c r="C10" s="2" t="inlineStr">
+        <is>
+          <t>PEDY</t>
+        </is>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" s="2" t="inlineStr">
+        <is>
+          <t>BY_STB COGIC_M27/613</t>
+        </is>
+      </c>
+      <c r="B11" s="2" t="n">
+        <v>1</v>
+      </c>
+      <c r="C11" s="2" t="inlineStr">
+        <is>
+          <t>STB COGIC</t>
+        </is>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" s="2" t="inlineStr">
+        <is>
+          <t>BY_T2HB DENON_SP1B/30</t>
+        </is>
+      </c>
+      <c r="B12" s="2" t="n">
+        <v>1</v>
+      </c>
+      <c r="C12" s="2" t="inlineStr">
+        <is>
+          <t>T2HB DENON</t>
+        </is>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" s="2" t="inlineStr">
+        <is>
+          <t>HZ_EXOTIC_1B</t>
+        </is>
+      </c>
+      <c r="B13" s="2" t="n">
+        <v>1</v>
+      </c>
+      <c r="C13" s="2" t="inlineStr">
+        <is>
+          <t>IDPEXO</t>
+        </is>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" s="2" t="inlineStr">
+        <is>
+          <t>HZ_HAYLIE_1B</t>
+        </is>
+      </c>
+      <c r="B14" s="2" t="n">
+        <v>1</v>
+      </c>
+      <c r="C14" s="2" t="inlineStr">
+        <is>
+          <t>IBBHAY</t>
+        </is>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" s="2" t="inlineStr">
+        <is>
+          <t>HZ_IDPWKS24_2</t>
+        </is>
+      </c>
+      <c r="B15" s="2" t="n">
+        <v>2</v>
+      </c>
+      <c r="C15" s="2" t="inlineStr">
+        <is>
+          <t>IDPWKS24IDPWKS24</t>
+        </is>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" s="2" t="inlineStr">
+        <is>
+          <t>HZ_MILEY_1B</t>
+        </is>
+      </c>
+      <c r="B16" s="2" t="n">
+        <v>1</v>
+      </c>
+      <c r="C16" s="2" t="inlineStr">
+        <is>
+          <t>HEFMIL</t>
+        </is>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" s="2" t="inlineStr">
+        <is>
+          <t>HZ_SB2XB48_3T2/30/27</t>
+        </is>
+      </c>
+      <c r="B17" s="2" t="n">
+        <v>2</v>
+      </c>
+      <c r="C17" s="2" t="inlineStr">
+        <is>
+          <t>SB2XB48</t>
+        </is>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" s="2" t="inlineStr">
+        <is>
+          <t>HZ_VOGUE CROP_1B</t>
+        </is>
+      </c>
+      <c r="B18" s="2" t="n">
+        <v>1</v>
+      </c>
+      <c r="C18" s="2" t="inlineStr">
+        <is>
+          <t>IHBVCR</t>
+        </is>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" s="2" t="inlineStr">
+        <is>
+          <t>OT_ PQWPNBF42_DR2T1B/2730</t>
+        </is>
+      </c>
+      <c r="B19" s="2" t="n">
+        <v>1</v>
+      </c>
+      <c r="C19" s="2" t="inlineStr">
+        <is>
+          <t>PQWPNBF42</t>
+        </is>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" s="2" t="inlineStr">
+        <is>
+          <t>OT_3C WHIRLY LOOP_2</t>
+        </is>
+      </c>
+      <c r="B20" s="2" t="n">
+        <v>10</v>
+      </c>
+      <c r="C20" s="2" t="inlineStr">
+        <is>
+          <t>KXBIW</t>
+        </is>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" s="2" t="inlineStr">
+        <is>
+          <t>OT_DUVESSA REMI YAKI 16_LT1B/433</t>
+        </is>
+      </c>
+      <c r="B21" s="2" t="n">
+        <v>4</v>
+      </c>
+      <c r="C21" s="2" t="inlineStr">
+        <is>
+          <t>HWDVY16</t>
+        </is>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" s="2" t="inlineStr">
+        <is>
+          <t>OT_GOLD OCEAN BODY 16-18-20_NBLK</t>
+        </is>
+      </c>
+      <c r="B22" s="2" t="n">
+        <v>1</v>
+      </c>
+      <c r="C22" s="2" t="inlineStr">
+        <is>
+          <t>HWMGO161820</t>
+        </is>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" s="2" t="inlineStr">
+        <is>
+          <t>OT_LUXELINE NATURAL BODY 10_NBLK</t>
+        </is>
+      </c>
+      <c r="B23" s="2" t="n">
+        <v>2</v>
+      </c>
+      <c r="C23" s="2" t="inlineStr">
+        <is>
+          <t>HWLLNB10</t>
+        </is>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" s="2" t="inlineStr">
+        <is>
+          <t>OT_ROLL UP 44PCS_280</t>
+        </is>
+      </c>
+      <c r="B24" s="2" t="n">
+        <v>1</v>
+      </c>
+      <c r="C24" s="2" t="inlineStr">
+        <is>
+          <t>HWVBRU234</t>
+        </is>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" s="2" t="inlineStr">
+        <is>
+          <t>OT_ROLL UP 44PCS_33</t>
+        </is>
+      </c>
+      <c r="B25" s="2" t="n">
+        <v>1</v>
+      </c>
+      <c r="C25" s="2" t="inlineStr">
+        <is>
+          <t>HWVBRU234</t>
+        </is>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26" s="2" t="inlineStr">
+        <is>
           <t>OT_ROLL UP 44PCS_4</t>
         </is>
       </c>
-      <c r="B10" s="2" t="n">
-        <v>1</v>
-      </c>
-      <c r="C10" s="2" t="inlineStr">
+      <c r="B26" s="2" t="n">
+        <v>1</v>
+      </c>
+      <c r="C26" s="2" t="inlineStr">
         <is>
           <t>HWVBRU234</t>
+        </is>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27" s="2" t="inlineStr">
+        <is>
+          <t>OT_SPIRALLY_4</t>
+        </is>
+      </c>
+      <c r="B27" s="2" t="n">
+        <v>1</v>
+      </c>
+      <c r="C27" s="2" t="inlineStr">
+        <is>
+          <t>HWPBSP5</t>
+        </is>
+      </c>
+    </row>
+    <row r="28">
+      <c r="A28" s="2" t="inlineStr">
+        <is>
+          <t>OT_TOYA_1</t>
+        </is>
+      </c>
+      <c r="B28" s="2" t="n">
+        <v>2</v>
+      </c>
+      <c r="C28" s="2" t="inlineStr">
+        <is>
+          <t>QPNTOYQPNTOY</t>
+        </is>
+      </c>
+    </row>
+    <row r="29">
+      <c r="A29" s="2" t="inlineStr">
+        <is>
+          <t>VF_BRIE-V_99J</t>
+        </is>
+      </c>
+      <c r="B29" s="2" t="n">
+        <v>1</v>
+      </c>
+      <c r="C29" s="2" t="inlineStr">
+        <is>
+          <t>45614</t>
+        </is>
+      </c>
+    </row>
+    <row r="30">
+      <c r="A30" s="2" t="inlineStr">
+        <is>
+          <t>VF_ELSIE_613</t>
+        </is>
+      </c>
+      <c r="B30" s="2" t="n">
+        <v>1</v>
+      </c>
+      <c r="C30" s="2" t="inlineStr">
+        <is>
+          <t>46700</t>
         </is>
       </c>
     </row>

</xml_diff>